<commit_message>
New ppt & instructions + data
</commit_message>
<xml_diff>
--- a/NewTasks/Subject Information Form.xlsx
+++ b/NewTasks/Subject Information Form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubing/Desktop/NewTasks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEA889D5-214B-674F-91FA-61DF782D01AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8919B4-776A-D444-A22A-F21D7E50AA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{70FF539A-39A6-884F-AFE5-D1160AC3BE7C}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15580" xr2:uid="{70FF539A-39A6-884F-AFE5-D1160AC3BE7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Subject Information</t>
   </si>
@@ -75,29 +75,68 @@
     <t>Daris ID</t>
   </si>
   <si>
-    <t>Scan Date</t>
-  </si>
-  <si>
-    <t>Scan Time</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Subject Assent/Consent</t>
   </si>
   <si>
-    <t>Ö</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Sound wasn't on for the safty tasks</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>8:00-10:10</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Olivia Hedge </t>
+  </si>
+  <si>
+    <t>mkcoates@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Maddy Coates</t>
+  </si>
+  <si>
+    <t>olivia.hedge@gmail.com</t>
+  </si>
+  <si>
+    <t>whiteantsrule@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Ryan White</t>
+  </si>
+  <si>
+    <t>Ethan White</t>
+  </si>
+  <si>
+    <t>Actural Scan Time</t>
+  </si>
+  <si>
+    <t>Actural Scan Date</t>
+  </si>
+  <si>
+    <t>Scheduled Starting Time</t>
+  </si>
+  <si>
+    <t>Scheduled Scan Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,12 +150,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,8 +190,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,16 +213,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,106 +534,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8C016-3E65-4B43-A673-F6E7DA8E8F02}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="17.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="5" customWidth="1"/>
-    <col min="11" max="13" width="11.83203125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="54" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="9.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="25.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="17.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="3" customWidth="1"/>
+    <col min="13" max="14" width="20.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="37.6640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="11.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="2"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="10">
+        <v>45274</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="4">
+        <v>45274</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>18</v>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="10">
+        <v>45306</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="10">
+        <v>45306</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="10">
+        <v>45315</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.10416666666666667</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="G1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>